<commit_message>
global mistaken subjects are fixed, need .pdf conclusion
</commit_message>
<xml_diff>
--- a/Excel/test_counter_1.xlsx
+++ b/Excel/test_counter_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\cpp_solutions\DaAA_IHW1\daaa-ihw1\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55D28E8-34C4-4CF0-992E-A7275B3B06ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D17F29-710E-46CB-BB28-7BB07D75C38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1068,7 +1068,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>8075</v>
+        <v>8087</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1082,7 +1082,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3">
-        <v>22754</v>
+        <v>22610</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1096,7 +1096,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3">
-        <v>20493</v>
+        <v>19926</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1110,7 +1110,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <v>14844</v>
+        <v>14596</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1124,7 +1124,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>6021</v>
+        <v>5781</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1138,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="3">
-        <v>6591</v>
+        <v>6107</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1152,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="3">
-        <v>1920</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1180,7 +1180,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="3">
-        <v>7263</v>
+        <v>7273</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1194,7 +1194,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="3">
-        <v>2904</v>
+        <v>2762</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1208,7 +1208,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="3">
-        <v>6551</v>
+        <v>6674</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1222,7 +1222,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="3">
-        <v>3383</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1236,7 +1236,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="3">
-        <v>3623</v>
+        <v>3678</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1250,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>8170</v>
+        <v>8124</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1264,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="3">
-        <v>23264</v>
+        <v>23222</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1278,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="3">
-        <v>19891</v>
+        <v>23832</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1292,7 +1292,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="3">
-        <v>15172</v>
+        <v>15698</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1306,7 +1306,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="3">
-        <v>6871</v>
+        <v>6801</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1320,7 +1320,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="3">
-        <v>7412</v>
+        <v>7359</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1334,7 +1334,7 @@
         <v>7</v>
       </c>
       <c r="D21" s="3">
-        <v>57074</v>
+        <v>55626</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1362,7 +1362,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="3">
-        <v>7271</v>
+        <v>7269</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1376,7 +1376,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="3">
-        <v>2798</v>
+        <v>2694</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1390,7 +1390,7 @@
         <v>11</v>
       </c>
       <c r="D25" s="3">
-        <v>7352</v>
+        <v>7581</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1404,7 +1404,7 @@
         <v>12</v>
       </c>
       <c r="D26" s="3">
-        <v>4183</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1418,7 +1418,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="3">
-        <v>4485</v>
+        <v>4890</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1516,7 +1516,7 @@
         <v>7</v>
       </c>
       <c r="D34" s="3">
-        <v>10162</v>
+        <v>18744</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1614,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="3">
-        <v>8405</v>
+        <v>8547</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1628,7 +1628,7 @@
         <v>2</v>
       </c>
       <c r="D42" s="3">
-        <v>26816</v>
+        <v>26906</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1642,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="D43" s="3">
-        <v>28424</v>
+        <v>28529</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1656,7 +1656,7 @@
         <v>4</v>
       </c>
       <c r="D44" s="3">
-        <v>19899</v>
+        <v>20004</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1670,7 +1670,7 @@
         <v>5</v>
       </c>
       <c r="D45" s="3">
-        <v>12791</v>
+        <v>12941</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1684,7 +1684,7 @@
         <v>6</v>
       </c>
       <c r="D46" s="3">
-        <v>11548</v>
+        <v>11580</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1698,7 +1698,7 @@
         <v>7</v>
       </c>
       <c r="D47" s="3">
-        <v>2784</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1726,7 +1726,7 @@
         <v>9</v>
       </c>
       <c r="D49" s="3">
-        <v>7103</v>
+        <v>7091</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1740,7 +1740,7 @@
         <v>10</v>
       </c>
       <c r="D50" s="3">
-        <v>10253</v>
+        <v>11576</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1754,7 +1754,7 @@
         <v>11</v>
       </c>
       <c r="D51" s="3">
-        <v>6584</v>
+        <v>6514</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1768,7 +1768,7 @@
         <v>12</v>
       </c>
       <c r="D52" s="3">
-        <v>3445</v>
+        <v>3554</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1782,7 +1782,7 @@
         <v>13</v>
       </c>
       <c r="D53" s="4">
-        <v>3826</v>
+        <v>3878</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1796,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="D54" s="3">
-        <v>31154</v>
+        <v>31141</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1810,7 +1810,7 @@
         <v>2</v>
       </c>
       <c r="D55" s="3">
-        <v>91898</v>
+        <v>91148</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1824,7 +1824,7 @@
         <v>3</v>
       </c>
       <c r="D56" s="3">
-        <v>83642</v>
+        <v>73179</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1838,7 +1838,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="3">
-        <v>59347</v>
+        <v>56270</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1852,7 +1852,7 @@
         <v>5</v>
       </c>
       <c r="D58" s="3">
-        <v>22711</v>
+        <v>21461</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1866,7 +1866,7 @@
         <v>6</v>
       </c>
       <c r="D59" s="3">
-        <v>22048</v>
+        <v>20646</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1880,7 +1880,7 @@
         <v>7</v>
       </c>
       <c r="D60" s="3">
-        <v>3720</v>
+        <v>3724</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1908,7 +1908,7 @@
         <v>9</v>
       </c>
       <c r="D62" s="3">
-        <v>16349</v>
+        <v>16353</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1922,7 +1922,7 @@
         <v>10</v>
       </c>
       <c r="D63" s="3">
-        <v>8375</v>
+        <v>7860</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1936,7 +1936,7 @@
         <v>11</v>
       </c>
       <c r="D64" s="3">
-        <v>15234</v>
+        <v>15500</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1950,7 +1950,7 @@
         <v>12</v>
       </c>
       <c r="D65" s="3">
-        <v>7356</v>
+        <v>7469</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1964,7 +1964,7 @@
         <v>13</v>
       </c>
       <c r="D66" s="3">
-        <v>8984</v>
+        <v>9679</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1978,7 +1978,7 @@
         <v>1</v>
       </c>
       <c r="D67" s="3">
-        <v>31388</v>
+        <v>31401</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1992,7 +1992,7 @@
         <v>2</v>
       </c>
       <c r="D68" s="3">
-        <v>93488</v>
+        <v>95438</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -2006,7 +2006,7 @@
         <v>3</v>
       </c>
       <c r="D69" s="3">
-        <v>83899</v>
+        <v>92566</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -2020,7 +2020,7 @@
         <v>4</v>
       </c>
       <c r="D70" s="3">
-        <v>60925</v>
+        <v>64092</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -2034,7 +2034,7 @@
         <v>5</v>
       </c>
       <c r="D71" s="3">
-        <v>25361</v>
+        <v>28611</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -2048,7 +2048,7 @@
         <v>6</v>
       </c>
       <c r="D72" s="3">
-        <v>23934</v>
+        <v>26267</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -2062,7 +2062,7 @@
         <v>7</v>
       </c>
       <c r="D73" s="3">
-        <v>59352</v>
+        <v>59264</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2090,7 +2090,7 @@
         <v>9</v>
       </c>
       <c r="D75" s="3">
-        <v>16375</v>
+        <v>16369</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2104,7 +2104,7 @@
         <v>10</v>
       </c>
       <c r="D76" s="3">
-        <v>6343</v>
+        <v>6098</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2118,7 +2118,7 @@
         <v>11</v>
       </c>
       <c r="D77" s="3">
-        <v>17511</v>
+        <v>17205</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2132,7 +2132,7 @@
         <v>12</v>
       </c>
       <c r="D78" s="3">
-        <v>10110</v>
+        <v>10379</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2146,7 +2146,7 @@
         <v>13</v>
       </c>
       <c r="D79" s="3">
-        <v>12733</v>
+        <v>11994</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2244,7 +2244,7 @@
         <v>7</v>
       </c>
       <c r="D86" s="3">
-        <v>11962</v>
+        <v>20544</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="D93" s="3">
-        <v>32670</v>
+        <v>33347</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -2356,7 +2356,7 @@
         <v>2</v>
       </c>
       <c r="D94" s="3">
-        <v>108536</v>
+        <v>108806</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2370,7 +2370,7 @@
         <v>3</v>
       </c>
       <c r="D95" s="3">
-        <v>113440</v>
+        <v>114554</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2384,7 +2384,7 @@
         <v>4</v>
       </c>
       <c r="D96" s="3">
-        <v>79681</v>
+        <v>80004</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2398,7 +2398,7 @@
         <v>5</v>
       </c>
       <c r="D97" s="3">
-        <v>50441</v>
+        <v>50891</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -2412,7 +2412,7 @@
         <v>6</v>
       </c>
       <c r="D98" s="3">
-        <v>41587</v>
+        <v>41751</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -2426,7 +2426,7 @@
         <v>7</v>
       </c>
       <c r="D99" s="3">
-        <v>5298</v>
+        <v>5228</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2454,7 +2454,7 @@
         <v>9</v>
       </c>
       <c r="D101" s="3">
-        <v>15951</v>
+        <v>15919</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -2468,7 +2468,7 @@
         <v>10</v>
       </c>
       <c r="D102" s="3">
-        <v>31463</v>
+        <v>44401</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -2482,7 +2482,7 @@
         <v>11</v>
       </c>
       <c r="D103" s="3">
-        <v>15369</v>
+        <v>15551</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -2496,7 +2496,7 @@
         <v>12</v>
       </c>
       <c r="D104" s="3">
-        <v>8172</v>
+        <v>8411</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2510,7 +2510,7 @@
         <v>13</v>
       </c>
       <c r="D105" s="4">
-        <v>9555</v>
+        <v>9698</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -2524,7 +2524,7 @@
         <v>1</v>
       </c>
       <c r="D106" s="3">
-        <v>69216</v>
+        <v>69248</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2538,7 +2538,7 @@
         <v>2</v>
       </c>
       <c r="D107" s="3">
-        <v>209238</v>
+        <v>208230</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -2552,7 +2552,7 @@
         <v>3</v>
       </c>
       <c r="D108" s="3">
-        <v>175966</v>
+        <v>185581</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2566,7 +2566,7 @@
         <v>4</v>
       </c>
       <c r="D109" s="3">
-        <v>132442</v>
+        <v>133606</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -2580,7 +2580,7 @@
         <v>5</v>
       </c>
       <c r="D110" s="3">
-        <v>53061</v>
+        <v>51381</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -2594,7 +2594,7 @@
         <v>6</v>
       </c>
       <c r="D111" s="3">
-        <v>48829</v>
+        <v>47163</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -2608,7 +2608,7 @@
         <v>7</v>
       </c>
       <c r="D112" s="3">
-        <v>5520</v>
+        <v>5524</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -2636,7 +2636,7 @@
         <v>9</v>
       </c>
       <c r="D114" s="3">
-        <v>26128</v>
+        <v>26140</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="D115" s="3">
-        <v>15647</v>
+        <v>14650</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -2664,7 +2664,7 @@
         <v>11</v>
       </c>
       <c r="D116" s="3">
-        <v>24660</v>
+        <v>24761</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -2678,7 +2678,7 @@
         <v>12</v>
       </c>
       <c r="D117" s="3">
-        <v>12432</v>
+        <v>12344</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -2692,7 +2692,7 @@
         <v>13</v>
       </c>
       <c r="D118" s="3">
-        <v>15389</v>
+        <v>15760</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
       <c r="D119" s="3">
-        <v>69646</v>
+        <v>69657</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -2720,7 +2720,7 @@
         <v>2</v>
       </c>
       <c r="D120" s="3">
-        <v>213066</v>
+        <v>214128</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -2734,7 +2734,7 @@
         <v>3</v>
       </c>
       <c r="D121" s="3">
-        <v>200815</v>
+        <v>214044</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -2748,7 +2748,7 @@
         <v>4</v>
       </c>
       <c r="D122" s="3">
-        <v>140716</v>
+        <v>142980</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -2762,7 +2762,7 @@
         <v>5</v>
       </c>
       <c r="D123" s="3">
-        <v>59441</v>
+        <v>61211</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -2776,7 +2776,7 @@
         <v>6</v>
       </c>
       <c r="D124" s="3">
-        <v>51785</v>
+        <v>53077</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -2790,7 +2790,7 @@
         <v>7</v>
       </c>
       <c r="D125" s="3">
-        <v>61152</v>
+        <v>61064</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -2818,7 +2818,7 @@
         <v>9</v>
       </c>
       <c r="D127" s="3">
-        <v>26172</v>
+        <v>26168</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -2832,7 +2832,7 @@
         <v>10</v>
       </c>
       <c r="D128" s="3">
-        <v>10884</v>
+        <v>9936</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -2846,7 +2846,7 @@
         <v>11</v>
       </c>
       <c r="D129" s="3">
-        <v>28122</v>
+        <v>28040</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -2860,7 +2860,7 @@
         <v>12</v>
       </c>
       <c r="D130" s="3">
-        <v>16979</v>
+        <v>17048</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -2874,7 +2874,7 @@
         <v>13</v>
       </c>
       <c r="D131" s="3">
-        <v>20101</v>
+        <v>20395</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -2972,7 +2972,7 @@
         <v>7</v>
       </c>
       <c r="D138" s="3">
-        <v>13762</v>
+        <v>22344</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -3070,7 +3070,7 @@
         <v>1</v>
       </c>
       <c r="D145" s="3">
-        <v>72263</v>
+        <v>74397</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
@@ -3084,7 +3084,7 @@
         <v>2</v>
       </c>
       <c r="D146" s="3">
-        <v>245262</v>
+        <v>245706</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -3098,7 +3098,7 @@
         <v>3</v>
       </c>
       <c r="D147" s="3">
-        <v>257561</v>
+        <v>258079</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -3112,7 +3112,7 @@
         <v>4</v>
       </c>
       <c r="D148" s="3">
-        <v>179486</v>
+        <v>180004</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
@@ -3126,7 +3126,7 @@
         <v>5</v>
       </c>
       <c r="D149" s="3">
-        <v>113101</v>
+        <v>113841</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
@@ -3140,7 +3140,7 @@
         <v>6</v>
       </c>
       <c r="D150" s="3">
-        <v>89542</v>
+        <v>89818</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
@@ -3154,7 +3154,7 @@
         <v>7</v>
       </c>
       <c r="D151" s="3">
-        <v>7758</v>
+        <v>7828</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -3182,7 +3182,7 @@
         <v>9</v>
       </c>
       <c r="D153" s="3">
-        <v>25496</v>
+        <v>25410</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
@@ -3196,7 +3196,7 @@
         <v>10</v>
       </c>
       <c r="D154" s="3">
-        <v>72291</v>
+        <v>98476</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -3210,7 +3210,7 @@
         <v>11</v>
       </c>
       <c r="D155" s="3">
-        <v>25302</v>
+        <v>25229</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
@@ -3224,7 +3224,7 @@
         <v>12</v>
       </c>
       <c r="D156" s="3">
-        <v>13668</v>
+        <v>14110</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3238,7 +3238,7 @@
         <v>13</v>
       </c>
       <c r="D157" s="4">
-        <v>17047</v>
+        <v>17086</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
@@ -3252,7 +3252,7 @@
         <v>1</v>
       </c>
       <c r="D158" s="3">
-        <v>122311</v>
+        <v>122322</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
@@ -3266,7 +3266,7 @@
         <v>2</v>
       </c>
       <c r="D159" s="3">
-        <v>369746</v>
+        <v>370850</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
@@ -3280,7 +3280,7 @@
         <v>3</v>
       </c>
       <c r="D160" s="3">
-        <v>331964</v>
+        <v>328455</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
@@ -3294,7 +3294,7 @@
         <v>4</v>
       </c>
       <c r="D161" s="3">
-        <v>236679</v>
+        <v>237106</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
@@ -3308,7 +3308,7 @@
         <v>5</v>
       </c>
       <c r="D162" s="3">
-        <v>88691</v>
+        <v>90531</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
@@ -3322,7 +3322,7 @@
         <v>6</v>
       </c>
       <c r="D163" s="3">
-        <v>81998</v>
+        <v>81887</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
@@ -3336,7 +3336,7 @@
         <v>7</v>
       </c>
       <c r="D164" s="3">
-        <v>7320</v>
+        <v>7324</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
@@ -3364,7 +3364,7 @@
         <v>9</v>
       </c>
       <c r="D166" s="3">
-        <v>36452</v>
+        <v>36428</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
@@ -3378,7 +3378,7 @@
         <v>10</v>
       </c>
       <c r="D167" s="3">
-        <v>25558</v>
+        <v>24521</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
@@ -3392,7 +3392,7 @@
         <v>11</v>
       </c>
       <c r="D168" s="3">
-        <v>33867</v>
+        <v>34443</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
@@ -3406,7 +3406,7 @@
         <v>12</v>
       </c>
       <c r="D169" s="3">
-        <v>17265</v>
+        <v>17827</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
@@ -3420,7 +3420,7 @@
         <v>13</v>
       </c>
       <c r="D170" s="3">
-        <v>21027</v>
+        <v>21739</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
@@ -3434,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="D171" s="3">
-        <v>122924</v>
+        <v>122961</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
@@ -3448,7 +3448,7 @@
         <v>2</v>
       </c>
       <c r="D172" s="3">
-        <v>376490</v>
+        <v>383738</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
@@ -3462,7 +3462,7 @@
         <v>3</v>
       </c>
       <c r="D173" s="3">
-        <v>367015</v>
+        <v>388263</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
@@ -3476,7 +3476,7 @@
         <v>4</v>
       </c>
       <c r="D174" s="3">
-        <v>247896</v>
+        <v>257028</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
@@ -3490,7 +3490,7 @@
         <v>5</v>
       </c>
       <c r="D175" s="3">
-        <v>99931</v>
+        <v>112011</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
@@ -3504,7 +3504,7 @@
         <v>6</v>
       </c>
       <c r="D176" s="3">
-        <v>84334</v>
+        <v>92827</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
@@ -3518,7 +3518,7 @@
         <v>7</v>
       </c>
       <c r="D177" s="3">
-        <v>62952</v>
+        <v>62864</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
@@ -3546,7 +3546,7 @@
         <v>9</v>
       </c>
       <c r="D179" s="3">
-        <v>36492</v>
+        <v>36526</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
@@ -3560,7 +3560,7 @@
         <v>10</v>
       </c>
       <c r="D180" s="3">
-        <v>15599</v>
+        <v>14663</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
@@ -3574,7 +3574,7 @@
         <v>11</v>
       </c>
       <c r="D181" s="3">
-        <v>39348</v>
+        <v>39592</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -3588,7 +3588,7 @@
         <v>12</v>
       </c>
       <c r="D182" s="3">
-        <v>24879</v>
+        <v>25491</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
@@ -3602,7 +3602,7 @@
         <v>13</v>
       </c>
       <c r="D183" s="3">
-        <v>29297</v>
+        <v>28984</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -3700,7 +3700,7 @@
         <v>7</v>
       </c>
       <c r="D190" s="3">
-        <v>15562</v>
+        <v>24144</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
@@ -3798,7 +3798,7 @@
         <v>1</v>
       </c>
       <c r="D197" s="3">
-        <v>127692</v>
+        <v>131697</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
@@ -3812,7 +3812,7 @@
         <v>2</v>
       </c>
       <c r="D198" s="3">
-        <v>437000</v>
+        <v>437606</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
@@ -3826,7 +3826,7 @@
         <v>3</v>
       </c>
       <c r="D199" s="3">
-        <v>458397</v>
+        <v>459104</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
@@ -3840,7 +3840,7 @@
         <v>4</v>
       </c>
       <c r="D200" s="3">
-        <v>319297</v>
+        <v>320004</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
@@ -3854,7 +3854,7 @@
         <v>5</v>
       </c>
       <c r="D201" s="3">
-        <v>200781</v>
+        <v>201791</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
@@ -3868,7 +3868,7 @@
         <v>6</v>
       </c>
       <c r="D202" s="3">
-        <v>155305</v>
+        <v>155693</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
@@ -3882,7 +3882,7 @@
         <v>7</v>
       </c>
       <c r="D203" s="3">
-        <v>10290</v>
+        <v>10428</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
@@ -3910,7 +3910,7 @@
         <v>9</v>
       </c>
       <c r="D205" s="3">
-        <v>35504</v>
+        <v>35408</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
@@ -3924,7 +3924,7 @@
         <v>10</v>
       </c>
       <c r="D206" s="3">
-        <v>130629</v>
+        <v>173801</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
@@ -3938,7 +3938,7 @@
         <v>11</v>
       </c>
       <c r="D207" s="3">
-        <v>35446</v>
+        <v>35496</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
@@ -3952,7 +3952,7 @@
         <v>12</v>
       </c>
       <c r="D208" s="3">
-        <v>18796</v>
+        <v>19433</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3966,7 +3966,7 @@
         <v>13</v>
       </c>
       <c r="D209" s="4">
-        <v>23058</v>
+        <v>23383</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
@@ -3980,7 +3980,7 @@
         <v>1</v>
       </c>
       <c r="D210" s="3">
-        <v>190386</v>
+        <v>190390</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
@@ -3994,7 +3994,7 @@
         <v>2</v>
       </c>
       <c r="D211" s="3">
-        <v>575390</v>
+        <v>579776</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
@@ -4008,7 +4008,7 @@
         <v>3</v>
       </c>
       <c r="D212" s="3">
-        <v>522361</v>
+        <v>507488</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
@@ -4022,7 +4022,7 @@
         <v>4</v>
       </c>
       <c r="D213" s="3">
-        <v>367381</v>
+        <v>368953</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
@@ -4036,7 +4036,7 @@
         <v>5</v>
       </c>
       <c r="D214" s="3">
-        <v>132881</v>
+        <v>140191</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
@@ -4050,7 +4050,7 @@
         <v>6</v>
       </c>
       <c r="D215" s="3">
-        <v>122606</v>
+        <v>125774</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
@@ -4064,7 +4064,7 @@
         <v>7</v>
       </c>
       <c r="D216" s="3">
-        <v>9120</v>
+        <v>9124</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
@@ -4092,7 +4092,7 @@
         <v>9</v>
       </c>
       <c r="D218" s="3">
-        <v>46708</v>
+        <v>46822</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
@@ -4106,7 +4106,7 @@
         <v>10</v>
       </c>
       <c r="D219" s="3">
-        <v>37360</v>
+        <v>36156</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
@@ -4120,7 +4120,7 @@
         <v>11</v>
       </c>
       <c r="D220" s="3">
-        <v>44595</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
@@ -4134,7 +4134,7 @@
         <v>12</v>
       </c>
       <c r="D221" s="3">
-        <v>22464</v>
+        <v>23127</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
@@ -4148,7 +4148,7 @@
         <v>13</v>
       </c>
       <c r="D222" s="3">
-        <v>25752</v>
+        <v>26090</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
@@ -4162,7 +4162,7 @@
         <v>1</v>
       </c>
       <c r="D223" s="3">
-        <v>191178</v>
+        <v>191238</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
@@ -4176,7 +4176,7 @@
         <v>2</v>
       </c>
       <c r="D224" s="3">
-        <v>587456</v>
+        <v>590780</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
@@ -4190,7 +4190,7 @@
         <v>3</v>
       </c>
       <c r="D225" s="3">
-        <v>576418</v>
+        <v>582295</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
@@ -4204,7 +4204,7 @@
         <v>4</v>
       </c>
       <c r="D226" s="3">
-        <v>385848</v>
+        <v>389851</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
@@ -4218,7 +4218,7 @@
         <v>5</v>
       </c>
       <c r="D227" s="3">
-        <v>152991</v>
+        <v>158531</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
@@ -4232,7 +4232,7 @@
         <v>6</v>
       </c>
       <c r="D228" s="3">
-        <v>125908</v>
+        <v>129757</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
@@ -4246,7 +4246,7 @@
         <v>7</v>
       </c>
       <c r="D229" s="3">
-        <v>64752</v>
+        <v>64694</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
@@ -4274,7 +4274,7 @@
         <v>9</v>
       </c>
       <c r="D231" s="3">
-        <v>46930</v>
+        <v>46900</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
@@ -4288,7 +4288,7 @@
         <v>10</v>
       </c>
       <c r="D232" s="3">
-        <v>19403</v>
+        <v>20091</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
@@ -4302,7 +4302,7 @@
         <v>11</v>
       </c>
       <c r="D233" s="3">
-        <v>50971</v>
+        <v>51125</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
@@ -4316,7 +4316,7 @@
         <v>12</v>
       </c>
       <c r="D234" s="3">
-        <v>32725</v>
+        <v>32884</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
@@ -4330,7 +4330,7 @@
         <v>13</v>
       </c>
       <c r="D235" s="3">
-        <v>33896</v>
+        <v>35876</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
@@ -4428,7 +4428,7 @@
         <v>7</v>
       </c>
       <c r="D242" s="3">
-        <v>17362</v>
+        <v>25944</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
@@ -4526,7 +4526,7 @@
         <v>1</v>
       </c>
       <c r="D249" s="3">
-        <v>198935</v>
+        <v>205247</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
@@ -4540,7 +4540,7 @@
         <v>2</v>
       </c>
       <c r="D250" s="3">
-        <v>683690</v>
+        <v>684506</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
@@ -4554,7 +4554,7 @@
         <v>3</v>
       </c>
       <c r="D251" s="3">
-        <v>716677</v>
+        <v>717629</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
@@ -4568,7 +4568,7 @@
         <v>4</v>
       </c>
       <c r="D252" s="3">
-        <v>499052</v>
+        <v>500004</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
@@ -4582,7 +4582,7 @@
         <v>5</v>
       </c>
       <c r="D253" s="3">
-        <v>313381</v>
+        <v>314741</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
@@ -4596,7 +4596,7 @@
         <v>6</v>
       </c>
       <c r="D254" s="3">
-        <v>238495</v>
+        <v>239068</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
@@ -4610,7 +4610,7 @@
         <v>7</v>
       </c>
       <c r="D255" s="3">
-        <v>12750</v>
+        <v>13028</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
@@ -4638,7 +4638,7 @@
         <v>9</v>
       </c>
       <c r="D257" s="3">
-        <v>45646</v>
+        <v>45520</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.3">
@@ -4652,7 +4652,7 @@
         <v>10</v>
       </c>
       <c r="D258" s="3">
-        <v>203649</v>
+        <v>270376</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.3">
@@ -4666,7 +4666,7 @@
         <v>11</v>
       </c>
       <c r="D259" s="3">
-        <v>46350</v>
+        <v>46480</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.3">
@@ -4680,7 +4680,7 @@
         <v>12</v>
       </c>
       <c r="D260" s="3">
-        <v>25038</v>
+        <v>25818</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4694,7 +4694,7 @@
         <v>13</v>
       </c>
       <c r="D261" s="4">
-        <v>30515</v>
+        <v>31230</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
@@ -4708,7 +4708,7 @@
         <v>1</v>
       </c>
       <c r="D262" s="3">
-        <v>273509</v>
+        <v>273519</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
@@ -4722,7 +4722,7 @@
         <v>2</v>
       </c>
       <c r="D263" s="3">
-        <v>830244</v>
+        <v>833430</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
@@ -4736,7 +4736,7 @@
         <v>3</v>
       </c>
       <c r="D264" s="3">
-        <v>748308</v>
+        <v>704045</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
@@ -4750,7 +4750,7 @@
         <v>4</v>
       </c>
       <c r="D265" s="3">
-        <v>529344</v>
+        <v>523451</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
@@ -4764,7 +4764,7 @@
         <v>5</v>
       </c>
       <c r="D266" s="3">
-        <v>192421</v>
+        <v>197731</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
@@ -4778,7 +4778,7 @@
         <v>6</v>
       </c>
       <c r="D267" s="3">
-        <v>175290</v>
+        <v>177603</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
@@ -4792,7 +4792,7 @@
         <v>7</v>
       </c>
       <c r="D268" s="3">
-        <v>10920</v>
+        <v>10924</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
@@ -4820,7 +4820,7 @@
         <v>9</v>
       </c>
       <c r="D270" s="3">
-        <v>57900</v>
+        <v>57926</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
@@ -4834,7 +4834,7 @@
         <v>10</v>
       </c>
       <c r="D271" s="3">
-        <v>49766</v>
+        <v>48200</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
@@ -4848,7 +4848,7 @@
         <v>11</v>
       </c>
       <c r="D272" s="3">
-        <v>54509</v>
+        <v>54367</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.3">
@@ -4862,7 +4862,7 @@
         <v>12</v>
       </c>
       <c r="D273" s="3">
-        <v>27821</v>
+        <v>28506</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.3">
@@ -4876,7 +4876,7 @@
         <v>13</v>
       </c>
       <c r="D274" s="3">
-        <v>35734</v>
+        <v>35579</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">
@@ -4890,7 +4890,7 @@
         <v>1</v>
       </c>
       <c r="D275" s="3">
-        <v>274484</v>
+        <v>274574</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.3">
@@ -4904,7 +4904,7 @@
         <v>2</v>
       </c>
       <c r="D276" s="3">
-        <v>848832</v>
+        <v>854094</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.3">
@@ -4918,7 +4918,7 @@
         <v>3</v>
       </c>
       <c r="D277" s="3">
-        <v>820373</v>
+        <v>812118</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.3">
@@ -4932,7 +4932,7 @@
         <v>4</v>
       </c>
       <c r="D278" s="3">
-        <v>557246</v>
+        <v>562014</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.3">
@@ -4946,7 +4946,7 @@
         <v>5</v>
       </c>
       <c r="D279" s="3">
-        <v>223401</v>
+        <v>232171</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.3">
@@ -4960,7 +4960,7 @@
         <v>6</v>
       </c>
       <c r="D280" s="3">
-        <v>179759</v>
+        <v>185715</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.3">
@@ -4974,7 +4974,7 @@
         <v>7</v>
       </c>
       <c r="D281" s="3">
-        <v>66794</v>
+        <v>66494</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.3">
@@ -5002,7 +5002,7 @@
         <v>9</v>
       </c>
       <c r="D283" s="3">
-        <v>58048</v>
+        <v>58046</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.3">
@@ -5016,7 +5016,7 @@
         <v>10</v>
       </c>
       <c r="D284" s="3">
-        <v>25478</v>
+        <v>22889</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.3">
@@ -5030,7 +5030,7 @@
         <v>11</v>
       </c>
       <c r="D285" s="3">
-        <v>63663</v>
+        <v>63568</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.3">
@@ -5044,7 +5044,7 @@
         <v>12</v>
       </c>
       <c r="D286" s="3">
-        <v>42212</v>
+        <v>40719</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.3">
@@ -5058,7 +5058,7 @@
         <v>13</v>
       </c>
       <c r="D287" s="3">
-        <v>46269</v>
+        <v>48033</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.3">
@@ -5156,7 +5156,7 @@
         <v>7</v>
       </c>
       <c r="D294" s="3">
-        <v>19162</v>
+        <v>27744</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.3">
@@ -5254,7 +5254,7 @@
         <v>1</v>
       </c>
       <c r="D301" s="3">
-        <v>286053</v>
+        <v>295047</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.3">
@@ -5268,7 +5268,7 @@
         <v>2</v>
       </c>
       <c r="D302" s="3">
-        <v>985416</v>
+        <v>986406</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.3">
@@ -5282,7 +5282,7 @@
         <v>3</v>
       </c>
       <c r="D303" s="3">
-        <v>1032499</v>
+        <v>1033654</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.3">
@@ -5296,7 +5296,7 @@
         <v>4</v>
       </c>
       <c r="D304" s="3">
-        <v>718849</v>
+        <v>720004</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.3">
@@ -5310,7 +5310,7 @@
         <v>5</v>
       </c>
       <c r="D305" s="3">
-        <v>451041</v>
+        <v>452691</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
@@ -5324,7 +5324,7 @@
         <v>6</v>
       </c>
       <c r="D306" s="3">
-        <v>339706</v>
+        <v>340427</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
@@ -5338,7 +5338,7 @@
         <v>7</v>
       </c>
       <c r="D307" s="3">
-        <v>15368</v>
+        <v>15628</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
@@ -5366,7 +5366,7 @@
         <v>9</v>
       </c>
       <c r="D309" s="3">
-        <v>56398</v>
+        <v>56220</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.3">
@@ -5380,7 +5380,7 @@
         <v>10</v>
       </c>
       <c r="D310" s="3">
-        <v>295033</v>
+        <v>388201</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.3">
@@ -5394,7 +5394,7 @@
         <v>11</v>
       </c>
       <c r="D311" s="3">
-        <v>57946</v>
+        <v>57930</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.3">
@@ -5408,7 +5408,7 @@
         <v>12</v>
       </c>
       <c r="D312" s="3">
-        <v>30247</v>
+        <v>31175</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5422,7 +5422,7 @@
         <v>13</v>
       </c>
       <c r="D313" s="4">
-        <v>40057</v>
+        <v>40166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>